<commit_message>
Small fixes NA and spells 1
</commit_message>
<xml_diff>
--- a/Level_3_to_be_deployed1.0/p_steps/Explanations.xlsx
+++ b/Level_3_to_be_deployed1.0/p_steps/Explanations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13695" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="Report_01_Study_population_ALL" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Calculation</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t xml:space="preserve">For the source and study population an ageband is assigned to the age at op_start_date. Moreover, the year of op_start_date is added for both tables. Than, for the source population the time between op_start_date and op_end_date is calculated while for the study population the time of inclusion is calculated as the time between start_follow_up (maximum date out of start_study_date, op_start_date + 365 days) and end_follow_up (minimum date out of end_study_date, op_end_date, date_creation, recommended_end_date and the date at which the age of 56 is reached). Eventually, the time difference in years from source and study population a is summed by year op_start_date and the ageband at op_start_date. In the table, the decline of PY source to PY study represents the lost follow_up time from the initial extraction to the follow_up time that is used for the study. </t>
+  </si>
+  <si>
+    <t>ALL_R_01_02_CompareToSource.csv</t>
+  </si>
+  <si>
+    <t>ALL_R_01_03_STUDYPOP.csv</t>
   </si>
 </sst>
 </file>
@@ -152,7 +158,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -168,9 +174,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -208,7 +214,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -280,7 +286,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -432,15 +438,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="114.42578125" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="93.7109375" customWidth="1"/>
+    <col min="3" max="3" width="108.28515625" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
   </cols>
   <sheetData>
@@ -482,10 +488,16 @@
       <c r="C3" t="s">
         <v>25</v>
       </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>